<commit_message>
Loops forever sends email when there's a change
</commit_message>
<xml_diff>
--- a/FromPython.xlsx
+++ b/FromPython.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="144">
   <si>
     <t>Links</t>
   </si>
@@ -37,144 +37,138 @@
     <t>CPU</t>
   </si>
   <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=165759&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=098337&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168330&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=168835&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172060&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=125229&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=140431&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172059&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168332&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168331&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168737&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=140951&amp;sid=pn2p08dnc5n9l0u5kbccrdfgb7</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137161&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=165760&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=170318&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=148888&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168745&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=160442&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168734&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=174063&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=168736&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=166353&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1912_1909&amp;item_id=170247&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=122694&amp;sid=msc91cj9hc3m00da2jsmutur43</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137135&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=169845&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=139381&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=172728&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137684&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=148889&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=121427&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1912_1911&amp;item_id=140839&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172058&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=151439&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=173776&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168333&amp;sid=7jt65jt4uh390aen8d0n461f41</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=161698&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=166352&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=165762&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=167885&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=123857&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=140851&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168426&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
-  </si>
-  <si>
-    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168427&amp;sid=19ee5oo31ul94g74762dk99jn2</t>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=165759&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168330&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=168835&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172060&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=125229&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=140431&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172059&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168331&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168332&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=169896&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168737&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=165760&amp;sid=1jhg5jhdfu3dk939s9jshlg0e7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=140951&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137161&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=148888&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168745&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=160442&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168734&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=174063&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1912_1909&amp;item_id=170247&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=169845&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=168736&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=166353&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_374&amp;item_id=122694&amp;sid=91prnt1rdv1ttshrf3hotq4lc7</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137135&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=139381&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=172728&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=137684&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1912_1911&amp;item_id=140839&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=172058&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=151439&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=148889&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=121427&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=173776&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168333&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710&amp;item_id=162340&amp;sid=d7tu4r6f4dftdgp1b1sktm1092</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=167885&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1924&amp;item_id=165762&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=166352&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=123857&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168426&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=140851&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
+  </si>
+  <si>
+    <t>https://www.canadacomputers.com/product_info.php?cPath=710_1925_1920_1923&amp;item_id=168427&amp;sid=8d9dgrke4rjfrtlbbnavhuntl5</t>
   </si>
   <si>
     <t>ASUS TUF Gaming Notebook  15.6'' FHD AMD Ryzen 5-4600H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10, TUF506IH-RS53</t>
   </si>
   <si>
-    <t>MSI GL62 6QF-1093CA Gaming Notebook  15.6" FHD(1920 x 1080) Intel i7-6700HQ(2.60GHz) 8GB DDR4, 1TB (SATA) 7200rpm  nVidia GeForce GTX 960M, 2GB GDDR5 DVD Super Multi BT4.0 Windows 10 Home</t>
-  </si>
-  <si>
     <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD AMD R5-4600H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10, AN515-44-R623 (NH.Q9GAA.002)</t>
   </si>
   <si>
@@ -193,27 +187,27 @@
     <t>ASUS TUF Gaming Notebook  15.6" FHD Intel Core i5-10300H  GTX 1650, 512GB SSD, 8GB DDR4  Windows 10, TUF506LH-DB51-CA</t>
   </si>
   <si>
+    <t>ACER Nitro 5 Gaming Notebook  15.6'' FHD Intel Core i5-10300H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10, AN515-55-59NW (NH.Q7MAA.007)</t>
+  </si>
+  <si>
     <t>Acer Nitro 5 Gaming Notebook  17.3'' FHD Intel Core i5-10300H  GTX 1650Ti, 8GB DDR4, 512GB SSD  Windows 10, AN517-52-59RD (NH.Q82AA.002)</t>
   </si>
   <si>
-    <t>ACER Nitro 5 Gaming Notebook  15.6'' FHD Intel Core i5-10300H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10, AN515-55-59NW (NH.Q7MAA.007)</t>
+    <t>HP Pavilion Gaming Laptop 15-dk1010ca,i5-10300H,8GB DDR4,256GB PCIe NVMe M.2 SSD</t>
   </si>
   <si>
     <t>MSI GF63 Thin Gaming Notebook  15.6" FHD IPS Intel Core i5-10300H  GTX 1650, 8GB DDR4, 512GB SSD  Win10, GF63 10SCXR-221CA</t>
   </si>
   <si>
+    <t>ASUS TUF Gaming Notebook  15.6'' FHD 144Hz AMD Ryzen7-4800H  GTX 1650, 16GB DDR4, 512GB SSD  Windows 10, TUF506IH-RS74</t>
+  </si>
+  <si>
     <t>MSI Gaming Notebook  15.6'' FHD 120Hz Intel Core i5-9300H  GTX 1660Ti, 8GB DDR4, 512GB SSD  Windows 10, GL65 9SD-056CA</t>
   </si>
   <si>
     <t>ASUS TUF Gaming Notebook  15.6" FHD AMD Ryzen 7-3750H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10, FX505DT-EB73</t>
   </si>
   <si>
-    <t>ASUS TUF Gaming Notebook  15.6'' FHD 144Hz AMD Ryzen7-4800H  GTX 1650, 16GB DDR4, 512GB SSD  Windows 10, TUF506IH-RS74</t>
-  </si>
-  <si>
-    <t>PLANNING SKU BI PAVILION GAMING LAPTOP 15-DK1010CA</t>
-  </si>
-  <si>
     <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD Intel Core i5-9300H  GTX 1650, 8GB DDR4, 256GB SSD  Windows 10, AN515-54-56WT (NH.Q5UAA.004)</t>
   </si>
   <si>
@@ -229,24 +223,24 @@
     <t>HP Pavilion Gaming Laptop 16-a0010ca,i5-10300H,8GB DDR4 (2 X 4GB),256GB PCIe NVM</t>
   </si>
   <si>
+    <t>MSI GF63 Thin Gaming Notebook  15.6" 120Hz Intel Core i5-9300H  GTX1650Ti Max-Q, 16GB DDR4, 512GB SSD  Win10 Bilingual, GF63 9SCSR-432CA</t>
+  </si>
+  <si>
+    <t>Lenovo Legion 5 Gaming Notebook  15.6" FHD AMD Ryzen 7-4800H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10 Home, 82B5001AUS</t>
+  </si>
+  <si>
     <t>Lenovo IdeaPad L340 Gaming Notebook  17.3" FHD Intel Core i7-9750H  GTX 1650, 8GB RAM, 512GB SSD  Windows 10 Home, 81LL00AGUS</t>
   </si>
   <si>
     <t>MSI GF63 Thin Gaming Notebook  15.6" FHD IPS Intel Core i7-10750H  GTX1650, 16GB DDR4, 512GB SSD  Win10, GF63 10SCXR-086CA</t>
   </si>
   <si>
-    <t>MSI GF63 Thin Gaming Notebook  15.6" 120Hz Intel Core i5-9300H  GTX1650Ti Max-Q, 16GB DDR4, 512GB SSD  Win10 Bilingual, GF63 9SCSR-432CA</t>
-  </si>
-  <si>
     <t>Acer Predator Triton 700 (Refurbished) Notebook  15.6" FHD Intel Core i7-7700HQ  16GB DDR4, 512GB SSD,  GTX 1060   Windows 10, PT715-51-761M, (RNB-NH.Q2KAA.001)</t>
   </si>
   <si>
     <t>MSI Thin Gaming Notebook  15.6" FHD Intel Core i5-9300H  GTX 1650, 8GB DDR4, 256GB SSD  Windows 10, GF63 9SC-060CA</t>
   </si>
   <si>
-    <t>Lenovo Legion 5 Gaming Notebook  15.6" FHD AMD Ryzen 7-4800H  GTX 1650, 8GB DDR4, 512GB SSD  Windows 10 Home, 82B5001AUS</t>
-  </si>
-  <si>
     <t>Acer Gaming Notebook  17.3" FHD Intel i5 9300H  GTX 1650, 8 GB DDR4, 512GB PCIe SSD  Windows 10, AN517-51-59QP (NH.Q5WAA.003)</t>
   </si>
   <si>
@@ -256,21 +250,21 @@
     <t>MSI Gaming Notebook  15.6" FHD, Intel Core i7-8750H  GTX 1050Ti, 12GB DDR4, 128GB SSD, 1TB HDD  Win 10, GF63 8RD-412CA</t>
   </si>
   <si>
+    <t>Asus Vivobook K571 Gaming Notebook  15.6” FHD, Intel Core i7-9750H  GTX 1650, 16GB DDR4, 256GB SSD + 1TB HDD  Windows 10 Home, K571GT-EB76</t>
+  </si>
+  <si>
+    <t>ASUS TUF Gaming Notebook  15.6'' FHD Intel Core i7-10750H  GTX 1650Ti, 512 GB SSD, 8 GB DDR4  Windows 10, TUF506LI-DB71CA</t>
+  </si>
+  <si>
+    <t>MSI Alpha 15 Gaming Notebook  15.6" FHD AMD Ryzen7-3750H  16GB DDR4, 512GB SSD, AMD Redeon RX5500M  Win 10, A3DDK-012CA</t>
+  </si>
+  <si>
     <t>Acer Predator Helios 300 Gaming Notebook  15.6'' FHD Intel Core i5-9300H  RTX 2060, 8GB DDR4, 512GB SSD  Windows 10, PH315-52-563Q (NH.Q54AA.004)</t>
   </si>
   <si>
     <t>ASUS ROG Strix GL503GE-RS71 Scar Edition Gaming Notebook  15.6" (1920x1080) 120Hz  Intel i7-8750H (2.20 GHz)  8GB DDR4, 1TB SSHD (8GB Cache), NVIDIA GTX 1050Ti 4GB  Windows 10</t>
   </si>
   <si>
-    <t>Asus Vivobook K571 Gaming Notebook  15.6” FHD, Intel Core i7-9750H  GTX 1650, 16GB DDR4, 256GB SSD + 1TB HDD  Windows 10 Home, K571GT-EB76</t>
-  </si>
-  <si>
-    <t>ASUS TUF Gaming Notebook  15.6'' FHD Intel Core i7-10750H  GTX 1650Ti, 512 GB SSD, 8 GB DDR4  Windows 10, TUF506LI-DB71CA</t>
-  </si>
-  <si>
-    <t>MSI Alpha 15 Gaming Notebook  15.6" FHD AMD Ryzen7-3750H  16GB DDR4, 512GB SSD, AMD Redeon RX5500M  Win 10, A3DDK-012CA</t>
-  </si>
-  <si>
     <t>Acer Nitro 5 Gaming Notebook  15.6" FHD 144Hz Intel Core i5-10300H  GTX 1660Ti, 8GB DDR4, 512GB SSD  Windows 10, AN515-55-57Y8 (NH.Q7PAA.003)</t>
   </si>
   <si>
@@ -280,33 +274,30 @@
     <t>HP Pavilion Gaming 15-dk0000 15-dk0010nr 15.6" Gaming Notebook - 1920 x 1080 - Intel Core i5 (9th Gen) i5-9300H Quad-core (4 Core) 2.40 GHz - 8 GB RAM - 256 GB SSD - Shadow Black, Green Chrome - Windows 10 Home - NVIDIA GeForce GTX 1050 with 3 GB - In-pla</t>
   </si>
   <si>
+    <t>Lenovo Legion Y540 Powerful Ultra-slim Gaming Notebook  15.6'' FHD Intel Core i7-9750H  GTX 1660Ti, 16GB DDR4, 512GB SSD  Windows 10, 81SX00R8CC</t>
+  </si>
+  <si>
+    <t>ASUS TUF Gaming Notebook  17.3'' FHD 120Hz AMD Ryzen 7-4800H  GTX 1660Ti, 16GB DDR4, 1TB SSD  Windows 10, TUF706IU-AS76</t>
+  </si>
+  <si>
     <t>MSI GF65 Thin Gaming Notebook  15.6" 120Hz FHD IPS Intel Core i7-9750H  RTX2060, 16GB DDR4, 512GB SSD  Win10, GF65 9SEXR-436CA</t>
   </si>
   <si>
-    <t>ASUS TUF Gaming Notebook  17.3'' FHD 120Hz AMD Ryzen 7-4800H  GTX 1660Ti, 16GB DDR4, 1TB SSD  Windows 10, TUF706IU-AS76</t>
-  </si>
-  <si>
-    <t>Lenovo Legion Y540 Powerful Ultra-slim Gaming Notebook  15.6'' FHD Intel Core i7-9750H  GTX 1660Ti, 16GB DDR4, 512GB SSD  Windows 10, 81SX00R8CC</t>
-  </si>
-  <si>
     <t>Acer Nitro 5 Spin NP515-51-80XS Gaming Notebook NH.Q2YAA.004 15.6'' FHD (1920x1080)  Intel Core i7-8550U (1.8GHz)  8GB DDR4, 1TB HDD, 256GB SSD  NVIDIA GeForce GTX 1050  Windows 10 Home</t>
   </si>
   <si>
+    <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD 144Hz, Intel Core i5-9300H  RTX 2060, 16GB DDR4, 512GB SSD  Windows 10, AN515-54-547D (NH.Q96AA.002)</t>
+  </si>
+  <si>
     <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD Intel Core i7-9750H  GTX 1650, 16GB DDR4, 512GB SSD  Windows 10, AN515-54-75UQ (NH.Q5UAA.002)</t>
   </si>
   <si>
-    <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD 144Hz, Intel Core i5-9300H  RTX 2060, 16GB DDR4, 512GB SSD  Windows 10, AN515-54-547D (NH.Q96AA.002)</t>
-  </si>
-  <si>
     <t>Acer Nitro 5 Gaming Notebook  15.6'' FHD 144Hz, Intel Core i7-9750H  RTX 2060, 16GB DDR4, 512GB SSD  Windows 10, AN515-54-70KK (NH.Q96AA.001)</t>
   </si>
   <si>
     <t>$899.00</t>
   </si>
   <si>
-    <t>$899.88</t>
-  </si>
-  <si>
     <t>$949.99</t>
   </si>
   <si>
@@ -322,15 +313,15 @@
     <t>$1,099.99</t>
   </si>
   <si>
+    <t>$1,127.70</t>
+  </si>
+  <si>
     <t>$1,169.00</t>
   </si>
   <si>
     <t>$1,199.00</t>
   </si>
   <si>
-    <t>$1,206.08</t>
-  </si>
-  <si>
     <t>$1,249.00</t>
   </si>
   <si>
@@ -364,7 +355,7 @@
     <t>$1,399.99</t>
   </si>
   <si>
-    <t>$1,417.81</t>
+    <t>$1,440.30</t>
   </si>
   <si>
     <t>$1,499.00</t>
@@ -385,6 +376,9 @@
     <t>$100.00</t>
   </si>
   <si>
+    <t>$97.50</t>
+  </si>
+  <si>
     <t>$30.00</t>
   </si>
   <si>
@@ -403,21 +397,21 @@
     <t>12gb</t>
   </si>
   <si>
+    <t>16gb</t>
+  </si>
+  <si>
+    <t>GTX 1650</t>
+  </si>
+  <si>
+    <t>GTX 1050</t>
+  </si>
+  <si>
+    <t>GTX 1060</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
-    <t>16gb</t>
-  </si>
-  <si>
-    <t>GTX 1650</t>
-  </si>
-  <si>
-    <t>GTX 1050</t>
-  </si>
-  <si>
-    <t>GTX 1060</t>
-  </si>
-  <si>
     <t>GTX 1660</t>
   </si>
   <si>
@@ -436,10 +430,10 @@
     <t>Intel 10300H</t>
   </si>
   <si>
+    <t>AMD 4800H</t>
+  </si>
+  <si>
     <t>AMD 3750H</t>
-  </si>
-  <si>
-    <t>AMD 4800H</t>
   </si>
   <si>
     <t>AMD 585H</t>
@@ -822,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -864,22 +858,22 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -890,22 +884,22 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -916,22 +910,22 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -942,22 +936,22 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -968,22 +962,22 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -994,22 +988,22 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1020,22 +1014,22 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1046,22 +1040,22 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1072,22 +1066,22 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1098,22 +1092,22 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
         <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
         <v>131</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1124,22 +1118,22 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1150,22 +1144,22 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1176,22 +1170,22 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1202,22 +1196,22 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1228,22 +1222,22 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H16" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1254,22 +1248,22 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G17" t="s">
         <v>131</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1280,22 +1274,22 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G18" t="s">
         <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1306,22 +1300,22 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1332,22 +1326,22 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
         <v>131</v>
       </c>
       <c r="H20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1358,22 +1352,22 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H21" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1384,22 +1378,22 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1410,22 +1404,22 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1436,22 +1430,22 @@
         <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1462,22 +1456,22 @@
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1488,22 +1482,22 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1514,22 +1508,22 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H27" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1540,16 +1534,16 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G28" t="s">
         <v>131</v>
@@ -1566,22 +1560,22 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
         <v>129</v>
       </c>
       <c r="H29" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1592,22 +1586,22 @@
         <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
         <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1618,22 +1612,22 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G31" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1644,22 +1638,22 @@
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H32" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1670,22 +1664,22 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E33" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H33" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1696,22 +1690,22 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1722,22 +1716,22 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H35" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1748,22 +1742,22 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1774,22 +1768,22 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F37" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H37" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1800,22 +1794,22 @@
         <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G38" t="s">
         <v>132</v>
       </c>
       <c r="H38" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1826,22 +1820,22 @@
         <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H39" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1852,19 +1846,19 @@
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H40" t="s">
         <v>141</v>
@@ -1878,22 +1872,22 @@
         <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H41" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1904,22 +1898,22 @@
         <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H42" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1930,22 +1924,22 @@
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1956,48 +1950,22 @@
         <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" t="s">
         <v>119</v>
       </c>
-      <c r="E44" t="s">
-        <v>120</v>
-      </c>
       <c r="F44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H44" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" t="s">
-        <v>128</v>
-      </c>
-      <c r="G45" t="s">
-        <v>135</v>
-      </c>
-      <c r="H45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2045,7 +2013,6 @@
     <hyperlink ref="B42" r:id="rId41"/>
     <hyperlink ref="B43" r:id="rId42"/>
     <hyperlink ref="B44" r:id="rId43"/>
-    <hyperlink ref="B45" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>